<commit_message>
-Mapear pessoas por turnos -Garantir 2 pessoas de cada departamento sempre
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruipe\Desktop\jeec\schedule_otimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74508CE3-C691-4AE2-8BFF-E0A44C190050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9431BF94-A6C0-44DD-93BB-F891C9C80EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>Nome</t>
   </si>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,6 +571,105 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update, results to excel
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruipe\Desktop\jeec\schedule_otimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9431BF94-A6C0-44DD-93BB-F891C9C80EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFDB437-F0EB-4D99-A998-FFDE0D6B5CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="114">
   <si>
     <t>Nome</t>
   </si>
@@ -47,55 +47,334 @@
     <t>Disponibilidade</t>
   </si>
   <si>
-    <t>Rui</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Afonso</t>
-  </si>
-  <si>
     <t>Webdev</t>
   </si>
   <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mariana </t>
-  </si>
-  <si>
-    <t>Joana</t>
-  </si>
-  <si>
-    <t>Gonçalo</t>
-  </si>
-  <si>
-    <t>Miguel</t>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Nome1</t>
+  </si>
+  <si>
+    <t>Nome2</t>
+  </si>
+  <si>
+    <t>Nome3</t>
+  </si>
+  <si>
+    <t>Nome4</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,1,1,1,1,1]</t>
   </si>
   <si>
     <t>[1,1,0,1,1,1,1,1,1,1]</t>
   </si>
   <si>
-    <t>[1,1,0,1,0,0,1,1,1,1]</t>
+    <t>[1,1,1,1,1,1,1,1,0,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,0,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,1,0,1,1,1]</t>
   </si>
   <si>
     <t>[1,1,1,1,0,1,1,1,0,1]</t>
   </si>
   <si>
-    <t>[1,1,1,1,1,0,1,1,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,1,1,1,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,1,1,1,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>Speakers</t>
+    <t>[1,1,0,1,1,0,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,1,1,0,1]</t>
+  </si>
+  <si>
+    <t>Nome5</t>
+  </si>
+  <si>
+    <t>Nome6</t>
+  </si>
+  <si>
+    <t>Nome7</t>
+  </si>
+  <si>
+    <t>Nome8</t>
+  </si>
+  <si>
+    <t>Nome9</t>
+  </si>
+  <si>
+    <t>Nome10</t>
+  </si>
+  <si>
+    <t>Nome11</t>
+  </si>
+  <si>
+    <t>Nome12</t>
+  </si>
+  <si>
+    <t>Nome13</t>
+  </si>
+  <si>
+    <t>Nome14</t>
+  </si>
+  <si>
+    <t>Nome15</t>
+  </si>
+  <si>
+    <t>Nome16</t>
+  </si>
+  <si>
+    <t>Nome17</t>
+  </si>
+  <si>
+    <t>Nome18</t>
+  </si>
+  <si>
+    <t>Nome19</t>
+  </si>
+  <si>
+    <t>Nome20</t>
+  </si>
+  <si>
+    <t>Nome21</t>
+  </si>
+  <si>
+    <t>Nome22</t>
+  </si>
+  <si>
+    <t>Nome23</t>
+  </si>
+  <si>
+    <t>Nome24</t>
+  </si>
+  <si>
+    <t>Nome25</t>
+  </si>
+  <si>
+    <t>Nome26</t>
+  </si>
+  <si>
+    <t>Nome27</t>
+  </si>
+  <si>
+    <t>Nome28</t>
+  </si>
+  <si>
+    <t>Nome29</t>
+  </si>
+  <si>
+    <t>Nome30</t>
+  </si>
+  <si>
+    <t>Nome31</t>
+  </si>
+  <si>
+    <t>Nome32</t>
+  </si>
+  <si>
+    <t>Nome33</t>
+  </si>
+  <si>
+    <t>Nome34</t>
+  </si>
+  <si>
+    <t>Nome35</t>
+  </si>
+  <si>
+    <t>Nome36</t>
+  </si>
+  <si>
+    <t>Nome37</t>
+  </si>
+  <si>
+    <t>Nome38</t>
+  </si>
+  <si>
+    <t>Nome39</t>
+  </si>
+  <si>
+    <t>Nome40</t>
+  </si>
+  <si>
+    <t>Nome41</t>
+  </si>
+  <si>
+    <t>Nome42</t>
+  </si>
+  <si>
+    <t>Nome43</t>
+  </si>
+  <si>
+    <t>Nome44</t>
+  </si>
+  <si>
+    <t>Nome45</t>
+  </si>
+  <si>
+    <t>Nome46</t>
+  </si>
+  <si>
+    <t>Nome47</t>
+  </si>
+  <si>
+    <t>Nome48</t>
+  </si>
+  <si>
+    <t>Nome49</t>
+  </si>
+  <si>
+    <t>Nome50</t>
+  </si>
+  <si>
+    <t>Nome51</t>
+  </si>
+  <si>
+    <t>Nome52</t>
+  </si>
+  <si>
+    <t>Nome53</t>
+  </si>
+  <si>
+    <t>Nome54</t>
+  </si>
+  <si>
+    <t>Nome55</t>
+  </si>
+  <si>
+    <t>Nome56</t>
+  </si>
+  <si>
+    <t>Nome57</t>
+  </si>
+  <si>
+    <t>Nome58</t>
+  </si>
+  <si>
+    <t>Nome59</t>
+  </si>
+  <si>
+    <t>Nome60</t>
+  </si>
+  <si>
+    <t>Nome61</t>
+  </si>
+  <si>
+    <t>Nome62</t>
+  </si>
+  <si>
+    <t>Nome63</t>
+  </si>
+  <si>
+    <t>Nome64</t>
+  </si>
+  <si>
+    <t>Nome65</t>
+  </si>
+  <si>
+    <t>Nome66</t>
+  </si>
+  <si>
+    <t>Nome67</t>
+  </si>
+  <si>
+    <t>Nome68</t>
+  </si>
+  <si>
+    <t>Nome69</t>
+  </si>
+  <si>
+    <t>Nome70</t>
+  </si>
+  <si>
+    <t>Nome71</t>
+  </si>
+  <si>
+    <t>Nome72</t>
+  </si>
+  <si>
+    <t>Nome73</t>
+  </si>
+  <si>
+    <t>Nome74</t>
+  </si>
+  <si>
+    <t>Nome75</t>
+  </si>
+  <si>
+    <t>Nome76</t>
+  </si>
+  <si>
+    <t>Nome77</t>
+  </si>
+  <si>
+    <t>Nome78</t>
+  </si>
+  <si>
+    <t>Nome79</t>
+  </si>
+  <si>
+    <t>Nome80</t>
+  </si>
+  <si>
+    <t>Nome81</t>
+  </si>
+  <si>
+    <t>Nome82</t>
+  </si>
+  <si>
+    <t>Nome83</t>
+  </si>
+  <si>
+    <t>Nome84</t>
+  </si>
+  <si>
+    <t>Nome85</t>
+  </si>
+  <si>
+    <t>Nome86</t>
+  </si>
+  <si>
+    <t>Nome87</t>
+  </si>
+  <si>
+    <t>Nome88</t>
+  </si>
+  <si>
+    <t>Nome89</t>
+  </si>
+  <si>
+    <t>Nome90</t>
+  </si>
+  <si>
+    <t>Nome91</t>
+  </si>
+  <si>
+    <t>Nome92</t>
+  </si>
+  <si>
+    <t>Nome93</t>
+  </si>
+  <si>
+    <t>Nome94</t>
+  </si>
+  <si>
+    <t>Nome95</t>
+  </si>
+  <si>
+    <t>Nome96</t>
+  </si>
+  <si>
+    <t>Nome97</t>
+  </si>
+  <si>
+    <t>Nome98</t>
+  </si>
+  <si>
+    <t>Nome99</t>
+  </si>
+  <si>
+    <t>Nome100</t>
   </si>
   <si>
     <t>Buss</t>
@@ -105,10 +384,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -450,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,203 +759,1106 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" t="s">
+        <v>113</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" t="s">
+        <v>113</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>107</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
equipas a aparecer nas pessoas
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruipe\Desktop\jeec\schedule_otimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E71CBA-8185-427D-8DA3-D1EF2198354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA1005E-3B63-4F71-9572-DE046680C3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
   <si>
     <t>Nome</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Disponibilidade</t>
   </si>
   <si>
-    <t>Webdev</t>
-  </si>
-  <si>
     <t>Speakers</t>
   </si>
   <si>
@@ -147,6 +144,81 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>WebDev</t>
+  </si>
+  <si>
+    <t>Nome31</t>
+  </si>
+  <si>
+    <t>Nome32</t>
+  </si>
+  <si>
+    <t>Nome33</t>
+  </si>
+  <si>
+    <t>Nome34</t>
+  </si>
+  <si>
+    <t>Nome35</t>
+  </si>
+  <si>
+    <t>Nome36</t>
+  </si>
+  <si>
+    <t>Nome37</t>
+  </si>
+  <si>
+    <t>Nome38</t>
+  </si>
+  <si>
+    <t>Nome39</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Coordinator</t>
+  </si>
+  <si>
+    <t>Nome40</t>
+  </si>
+  <si>
+    <t>Nome41</t>
+  </si>
+  <si>
+    <t>Nome42</t>
+  </si>
+  <si>
+    <t>Nome43</t>
+  </si>
+  <si>
+    <t>Nome44</t>
+  </si>
+  <si>
+    <t>Nome45</t>
+  </si>
+  <si>
+    <t>Nome46</t>
+  </si>
+  <si>
+    <t>Nome47</t>
+  </si>
+  <si>
+    <t>Nome48</t>
+  </si>
+  <si>
+    <t>Nome49</t>
+  </si>
+  <si>
+    <t>Nome50</t>
+  </si>
+  <si>
+    <t>Nome51</t>
+  </si>
+  <si>
+    <t>Business</t>
   </si>
 </sst>
 </file>
@@ -504,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,332 +600,563 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
         <v>3</v>
       </c>
-      <c r="C31" t="s">
-        <v>35</v>
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Turnos assimétricos (de dia para dia a existencia de turnos pode variar)
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruipe\Desktop\jeec\schedule_otimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2674C2E5-A086-4323-BBB7-F6FC514B71AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D30E52C-EC23-404F-9A3E-2E7A92E17B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$74</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="83">
   <si>
     <t>Nome</t>
   </si>
@@ -158,9 +161,6 @@
     <t>Nome33</t>
   </si>
   <si>
-    <t>Nome34</t>
-  </si>
-  <si>
     <t>Nome35</t>
   </si>
   <si>
@@ -179,12 +179,6 @@
     <t>Logistics</t>
   </si>
   <si>
-    <t>Coordinator</t>
-  </si>
-  <si>
-    <t>Nome40</t>
-  </si>
-  <si>
     <t>Nome41</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
     <t>Nome43</t>
   </si>
   <si>
-    <t>Nome44</t>
-  </si>
-  <si>
     <t>Nome45</t>
   </si>
   <si>
@@ -222,6 +213,81 @@
   </si>
   <si>
     <t>Volunteer</t>
+  </si>
+  <si>
+    <t>Nome52</t>
+  </si>
+  <si>
+    <t>Nome53</t>
+  </si>
+  <si>
+    <t>Nome54</t>
+  </si>
+  <si>
+    <t>Nome55</t>
+  </si>
+  <si>
+    <t>Nome56</t>
+  </si>
+  <si>
+    <t>Nome57</t>
+  </si>
+  <si>
+    <t>Nome58</t>
+  </si>
+  <si>
+    <t>Nome59</t>
+  </si>
+  <si>
+    <t>Nome61</t>
+  </si>
+  <si>
+    <t>Nome63</t>
+  </si>
+  <si>
+    <t>Nome65</t>
+  </si>
+  <si>
+    <t>Nome66</t>
+  </si>
+  <si>
+    <t>Nome67</t>
+  </si>
+  <si>
+    <t>Nome69</t>
+  </si>
+  <si>
+    <t>Nome74</t>
+  </si>
+  <si>
+    <t>Nome75</t>
+  </si>
+  <si>
+    <t>Nome76</t>
+  </si>
+  <si>
+    <t>Nome77</t>
+  </si>
+  <si>
+    <t>Nome78</t>
+  </si>
+  <si>
+    <t>Nome83</t>
+  </si>
+  <si>
+    <t>Nome86</t>
+  </si>
+  <si>
+    <t>Nome88</t>
+  </si>
+  <si>
+    <t>Nome89</t>
+  </si>
+  <si>
+    <t>Nome92</t>
+  </si>
+  <si>
+    <t>Nome94</t>
   </si>
 </sst>
 </file>
@@ -579,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:C78"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,10 +680,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -625,7 +691,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -636,7 +702,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -647,7 +713,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -658,10 +724,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -669,7 +735,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
@@ -680,10 +746,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -691,7 +757,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -702,7 +768,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
@@ -713,7 +779,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -724,7 +790,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -735,10 +801,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -746,10 +812,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
@@ -757,10 +823,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -768,10 +834,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -779,10 +845,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -790,10 +856,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -801,10 +867,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -812,10 +878,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -823,10 +889,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -834,7 +900,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -845,10 +911,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -856,10 +922,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -867,10 +933,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -878,10 +944,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
@@ -889,10 +955,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
@@ -900,10 +966,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
@@ -911,10 +977,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -922,10 +988,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
@@ -933,10 +999,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
@@ -944,10 +1010,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
@@ -955,10 +1021,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -966,10 +1032,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -977,10 +1043,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
@@ -988,10 +1054,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
@@ -999,10 +1065,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
         <v>34</v>
@@ -1010,10 +1076,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
@@ -1021,10 +1087,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
         <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -1032,10 +1098,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1043,10 +1109,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
         <v>34</v>
@@ -1054,10 +1120,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
         <v>34</v>
@@ -1065,10 +1131,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>34</v>
@@ -1076,10 +1142,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
         <v>34</v>
@@ -1087,10 +1153,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
         <v>34</v>
@@ -1098,10 +1164,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
         <v>34</v>
@@ -1109,10 +1175,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C48" t="s">
         <v>34</v>
@@ -1120,10 +1186,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
         <v>34</v>
@@ -1131,10 +1197,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C50" t="s">
         <v>34</v>
@@ -1142,10 +1208,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
         <v>34</v>
@@ -1153,16 +1219,263 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C52" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" t="s">
+        <v>57</v>
+      </c>
+      <c r="C64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:C74" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
2 novas regras + prep mega teste
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruipe\Desktop\jeec\schedule_otimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b68001cfe7d3a722/Ambiente de Trabalho/jeec/schedule_otimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D30E52C-EC23-404F-9A3E-2E7A92E17B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{5D30E52C-EC23-404F-9A3E-2E7A92E17B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64238208-0C0A-40E1-9F99-B8AD9B9A6CFD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="99">
   <si>
     <t>Nome</t>
   </si>
@@ -53,241 +53,289 @@
     <t>Speakers</t>
   </si>
   <si>
-    <t>Nome1</t>
-  </si>
-  <si>
-    <t>Nome2</t>
-  </si>
-  <si>
-    <t>Nome3</t>
-  </si>
-  <si>
-    <t>Nome4</t>
-  </si>
-  <si>
-    <t>Nome5</t>
-  </si>
-  <si>
-    <t>Nome6</t>
-  </si>
-  <si>
-    <t>Nome7</t>
-  </si>
-  <si>
-    <t>Nome8</t>
-  </si>
-  <si>
-    <t>Nome9</t>
-  </si>
-  <si>
-    <t>Nome10</t>
-  </si>
-  <si>
-    <t>Nome11</t>
-  </si>
-  <si>
-    <t>Nome12</t>
-  </si>
-  <si>
-    <t>Nome13</t>
-  </si>
-  <si>
-    <t>Nome14</t>
-  </si>
-  <si>
-    <t>Nome15</t>
-  </si>
-  <si>
-    <t>Nome16</t>
-  </si>
-  <si>
-    <t>Nome17</t>
-  </si>
-  <si>
-    <t>Nome18</t>
-  </si>
-  <si>
-    <t>Nome19</t>
-  </si>
-  <si>
-    <t>Nome20</t>
-  </si>
-  <si>
-    <t>Nome21</t>
-  </si>
-  <si>
-    <t>Nome22</t>
-  </si>
-  <si>
-    <t>Nome23</t>
-  </si>
-  <si>
-    <t>Nome24</t>
-  </si>
-  <si>
-    <t>Nome25</t>
-  </si>
-  <si>
-    <t>Nome26</t>
-  </si>
-  <si>
-    <t>Nome27</t>
-  </si>
-  <si>
-    <t>Nome28</t>
-  </si>
-  <si>
-    <t>Nome29</t>
-  </si>
-  <si>
-    <t>Nome30</t>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>WebDev</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>WD1</t>
+  </si>
+  <si>
+    <t>WD2</t>
+  </si>
+  <si>
+    <t>WD3</t>
+  </si>
+  <si>
+    <t>WD4</t>
+  </si>
+  <si>
+    <t>Bus1</t>
+  </si>
+  <si>
+    <t>Bus2</t>
+  </si>
+  <si>
+    <t>Bus3</t>
+  </si>
+  <si>
+    <t>Bus4</t>
+  </si>
+  <si>
+    <t>Log1</t>
+  </si>
+  <si>
+    <t>Log2</t>
+  </si>
+  <si>
+    <t>Log3</t>
+  </si>
+  <si>
+    <t>Sp1</t>
+  </si>
+  <si>
+    <t>Sp2</t>
+  </si>
+  <si>
+    <t>Sp3</t>
+  </si>
+  <si>
+    <t>Sp4</t>
+  </si>
+  <si>
+    <t>MK1</t>
+  </si>
+  <si>
+    <t>MK2</t>
+  </si>
+  <si>
+    <t>MK3</t>
+  </si>
+  <si>
+    <t>MK4</t>
+  </si>
+  <si>
+    <t>MK5</t>
+  </si>
+  <si>
+    <t>MK6</t>
+  </si>
+  <si>
+    <t>MK7</t>
+  </si>
+  <si>
+    <t>MK8</t>
+  </si>
+  <si>
+    <t>Vol1</t>
+  </si>
+  <si>
+    <t>Vol2</t>
+  </si>
+  <si>
+    <t>Vol3</t>
+  </si>
+  <si>
+    <t>Vol4</t>
+  </si>
+  <si>
+    <t>Vol5</t>
+  </si>
+  <si>
+    <t>Vol6</t>
+  </si>
+  <si>
+    <t>Vol7</t>
+  </si>
+  <si>
+    <t>Vol8</t>
+  </si>
+  <si>
+    <t>Vol9</t>
+  </si>
+  <si>
+    <t>Vol10</t>
+  </si>
+  <si>
+    <t>Vol11</t>
+  </si>
+  <si>
+    <t>Vol12</t>
+  </si>
+  <si>
+    <t>Vol13</t>
+  </si>
+  <si>
+    <t>Vol14</t>
+  </si>
+  <si>
+    <t>Vol15</t>
+  </si>
+  <si>
+    <t>Vol16</t>
+  </si>
+  <si>
+    <t>Vol17</t>
+  </si>
+  <si>
+    <t>WD5</t>
+  </si>
+  <si>
+    <t>WD6</t>
+  </si>
+  <si>
+    <t>WD7</t>
+  </si>
+  <si>
+    <t>WD8</t>
+  </si>
+  <si>
+    <t>WD9</t>
+  </si>
+  <si>
+    <t>Bus5</t>
+  </si>
+  <si>
+    <t>Bus6</t>
+  </si>
+  <si>
+    <t>Bus7</t>
+  </si>
+  <si>
+    <t>Bus8</t>
+  </si>
+  <si>
+    <t>Bus9</t>
+  </si>
+  <si>
+    <t>Bus10</t>
+  </si>
+  <si>
+    <t>Log4</t>
+  </si>
+  <si>
+    <t>Log5</t>
+  </si>
+  <si>
+    <t>Log6</t>
+  </si>
+  <si>
+    <t>Log7</t>
+  </si>
+  <si>
+    <t>Sp5</t>
+  </si>
+  <si>
+    <t>Sp6</t>
+  </si>
+  <si>
+    <t>Sp7</t>
+  </si>
+  <si>
+    <t>Vol18</t>
+  </si>
+  <si>
+    <t>Vol19</t>
+  </si>
+  <si>
+    <t>Vol20</t>
+  </si>
+  <si>
+    <t>Vol21</t>
+  </si>
+  <si>
+    <t>Vol22</t>
+  </si>
+  <si>
+    <t>Vol23</t>
+  </si>
+  <si>
+    <t>Vol24</t>
+  </si>
+  <si>
+    <t>Vol25</t>
+  </si>
+  <si>
+    <t>Vol26</t>
+  </si>
+  <si>
+    <t>Vol27</t>
+  </si>
+  <si>
+    <t>Vol28</t>
+  </si>
+  <si>
+    <t>Vol29</t>
+  </si>
+  <si>
+    <t>Vol30</t>
+  </si>
+  <si>
+    <t>Vol31</t>
+  </si>
+  <si>
+    <t>Vol32</t>
+  </si>
+  <si>
+    <t>Vol33</t>
+  </si>
+  <si>
+    <t>Vol34</t>
+  </si>
+  <si>
+    <t>Vol35</t>
+  </si>
+  <si>
+    <t>Vol36</t>
+  </si>
+  <si>
+    <t>Vol37</t>
+  </si>
+  <si>
+    <t>Vol38</t>
+  </si>
+  <si>
+    <t>Vol39</t>
+  </si>
+  <si>
+    <t>Vol40</t>
+  </si>
+  <si>
+    <t>Vol41</t>
+  </si>
+  <si>
+    <t>Vol42</t>
+  </si>
+  <si>
+    <t>Vol43</t>
+  </si>
+  <si>
+    <t>Vol44</t>
+  </si>
+  <si>
+    <t>Vol45</t>
+  </si>
+  <si>
+    <t>Vol46</t>
+  </si>
+  <si>
+    <t>Vol47</t>
+  </si>
+  <si>
+    <t>Vol48</t>
   </si>
   <si>
     <t>[1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>WebDev</t>
-  </si>
-  <si>
-    <t>Nome31</t>
-  </si>
-  <si>
-    <t>Nome32</t>
-  </si>
-  <si>
-    <t>Nome33</t>
-  </si>
-  <si>
-    <t>Nome35</t>
-  </si>
-  <si>
-    <t>Nome36</t>
-  </si>
-  <si>
-    <t>Nome37</t>
-  </si>
-  <si>
-    <t>Nome38</t>
-  </si>
-  <si>
-    <t>Nome39</t>
-  </si>
-  <si>
-    <t>Logistics</t>
-  </si>
-  <si>
-    <t>Nome41</t>
-  </si>
-  <si>
-    <t>Nome42</t>
-  </si>
-  <si>
-    <t>Nome43</t>
-  </si>
-  <si>
-    <t>Nome45</t>
-  </si>
-  <si>
-    <t>Nome46</t>
-  </si>
-  <si>
-    <t>Nome47</t>
-  </si>
-  <si>
-    <t>Nome48</t>
-  </si>
-  <si>
-    <t>Nome49</t>
-  </si>
-  <si>
-    <t>Nome50</t>
-  </si>
-  <si>
-    <t>Nome51</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Volunteer</t>
-  </si>
-  <si>
-    <t>Nome52</t>
-  </si>
-  <si>
-    <t>Nome53</t>
-  </si>
-  <si>
-    <t>Nome54</t>
-  </si>
-  <si>
-    <t>Nome55</t>
-  </si>
-  <si>
-    <t>Nome56</t>
-  </si>
-  <si>
-    <t>Nome57</t>
-  </si>
-  <si>
-    <t>Nome58</t>
-  </si>
-  <si>
-    <t>Nome59</t>
-  </si>
-  <si>
-    <t>Nome61</t>
-  </si>
-  <si>
-    <t>Nome63</t>
-  </si>
-  <si>
-    <t>Nome65</t>
-  </si>
-  <si>
-    <t>Nome66</t>
-  </si>
-  <si>
-    <t>Nome67</t>
-  </si>
-  <si>
-    <t>Nome69</t>
-  </si>
-  <si>
-    <t>Nome74</t>
-  </si>
-  <si>
-    <t>Nome75</t>
-  </si>
-  <si>
-    <t>Nome76</t>
-  </si>
-  <si>
-    <t>Nome77</t>
-  </si>
-  <si>
-    <t>Nome78</t>
-  </si>
-  <si>
-    <t>Nome83</t>
-  </si>
-  <si>
-    <t>Nome86</t>
-  </si>
-  <si>
-    <t>Nome88</t>
-  </si>
-  <si>
-    <t>Nome89</t>
-  </si>
-  <si>
-    <t>Nome92</t>
-  </si>
-  <si>
-    <t>Nome94</t>
   </si>
 </sst>
 </file>
@@ -346,6 +394,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -645,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91:C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,810 +721,986 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B72" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>82</v>
       </c>
-      <c r="B74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C74" t="s">
-        <v>34</v>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>96</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C74" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
+  <autoFilter ref="A1:C41" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C41">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
novo mega teste, com problema na distribuiçao final
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruipe\OneDrive\Ambiente de Trabalho\jeec\schedule_otimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b68001cfe7d3a722/Ambiente de Trabalho/jeec/schedule_otimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A974DD1-9F25-4430-90A8-4C5235FEE1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{DBA8300C-A3D3-4714-A3DA-56C05CC7D6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1951CEE-4384-462F-B586-DB75F0256B53}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
   <si>
     <t>Nome</t>
   </si>
@@ -71,18 +71,126 @@
     <t>WD1</t>
   </si>
   <si>
+    <t>WD2</t>
+  </si>
+  <si>
+    <t>WD3</t>
+  </si>
+  <si>
+    <t>WD4</t>
+  </si>
+  <si>
+    <t>WD5</t>
+  </si>
+  <si>
+    <t>WD6</t>
+  </si>
+  <si>
+    <t>WD7</t>
+  </si>
+  <si>
+    <t>WD8</t>
+  </si>
+  <si>
+    <t>WD9</t>
+  </si>
+  <si>
     <t>Bus1</t>
   </si>
   <si>
+    <t>Bus2</t>
+  </si>
+  <si>
+    <t>Bus3</t>
+  </si>
+  <si>
+    <t>Bus4</t>
+  </si>
+  <si>
+    <t>Bus5</t>
+  </si>
+  <si>
+    <t>Bus6</t>
+  </si>
+  <si>
+    <t>Bus7</t>
+  </si>
+  <si>
+    <t>Bus8</t>
+  </si>
+  <si>
+    <t>Bus9</t>
+  </si>
+  <si>
+    <t>Bus10</t>
+  </si>
+  <si>
     <t>Log1</t>
   </si>
   <si>
+    <t>Log2</t>
+  </si>
+  <si>
+    <t>Log3</t>
+  </si>
+  <si>
+    <t>Log4</t>
+  </si>
+  <si>
+    <t>Log5</t>
+  </si>
+  <si>
+    <t>Log6</t>
+  </si>
+  <si>
+    <t>Log7</t>
+  </si>
+  <si>
     <t>Sp1</t>
   </si>
   <si>
+    <t>Sp2</t>
+  </si>
+  <si>
+    <t>Sp3</t>
+  </si>
+  <si>
+    <t>Sp4</t>
+  </si>
+  <si>
+    <t>Sp5</t>
+  </si>
+  <si>
+    <t>Sp6</t>
+  </si>
+  <si>
+    <t>Sp7</t>
+  </si>
+  <si>
     <t>MK1</t>
   </si>
   <si>
+    <t>MK2</t>
+  </si>
+  <si>
+    <t>MK3</t>
+  </si>
+  <si>
+    <t>MK4</t>
+  </si>
+  <si>
+    <t>MK5</t>
+  </si>
+  <si>
+    <t>MK6</t>
+  </si>
+  <si>
+    <t>MK7</t>
+  </si>
+  <si>
+    <t>MK8</t>
+  </si>
+  <si>
     <t>Vol1</t>
   </si>
   <si>
@@ -140,9 +248,6 @@
     <t>Vol19</t>
   </si>
   <si>
-    <t>Bus10</t>
-  </si>
-  <si>
     <t>Vol20</t>
   </si>
   <si>
@@ -176,7 +281,223 @@
     <t>Vol30</t>
   </si>
   <si>
-    <t>[1,1,1,1,1,1,1]</t>
+    <t>[0,0,0,1,1,0,1,1,0,0,1,0,0,0,1,0,0,0,1,1,1,0,0,1,0,0,1,0,0,0,0,1,0,1,1,1,1,1,1,1,1,0,1,1,1,1,0,0,0,1,1,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,1,1,1,1,0,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,1,0,1,0,0,1,1,0,1,1,1,1,0,0,1,1,0,1,0,1,1,0,0,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,0,1,1,1,1,1,0,0,1,0,1,0,0,1,0,1,0,1,1,1,0,0,0,1,0,0,0,0,0,1,1,1,1,0,0,0,1,1,1,1,0,0,1,0,1,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,1,1,1,0,0,0,0,0,0,1,0,1,0,0,1,0,1,1,1,1,0,0,0,0,0,0,1,0,1,0,1,1,0,1,1,0,0,0,1,1,0,0,0,1,0,0,1,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,0,1,1,1,0,1,0,1,1,0,0,1,1,1,0,0,0,0,0,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,0,1,1,1,0,1,0,0,0,1,1,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,1,1,1,0,1,1,1,0,1,0,0,1,1,0,1,1,1,1,0,1,1,1,0,0,0,0,0,1,0,1,1,1,1,1,1,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,1,0,0,0,1,1,0,0,0,1,0,0,1,1,0,1,0,1,0,1,1,0,0,0,1,0,0,1,0,1,0,1,0,1,0,1,0,1,0,1,1,1,1,1,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,1,1,1,0,0,1,1,1,0,0,1,0,1,0,1,1,1,1,1,0,0,0,1,0,0,1,0,0,0,1,1,0,1,1,0,1,1,0,0,0,0,1,1,0,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,0,1,1,1,1,0,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,1,0,1,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,1,1,1,1,0,1,1,1,1,0,0,0,0,0,0,1,1,1,1,0,1,1,1,1,0,0,0,0,0,0,0,0,0,1,0,1,0,1,1,1,1,1,0,1,0,1,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,0,0,0,1,1,0,0,0,0,1,1,0,1,0,1,1,0,0,0,0,1,0,1,1,1,0,1,1,1,0,0,1,0,0,1,0,0,0,1,0,0,0,1,1,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,1,0,1,1,1,0,1,0,1,0,1,1,0,0,0,0,0,1,1,0,0,0,1,0,1,0,0,1,1,1,0,0,1,0,0,0,0,0,0,1,0,0,0,1,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,1,0,0,1,1,0,0,1,1,1,0,1,1,1,0,1,1,1,0,1,0,0,0,1,1,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,1,0,1,0,0,1,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,0,1,1,0,0,1,0,0,1,1,0,0,0,0,1,0,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,1,0,0,0,0,1,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,1,1,0,0,0,0,0,1,0,1,1,1,1,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,0,1,1,0,1,0,0,1,0,0,1,1,1,1,0,1,1,0,0,1,1,0,1,1,0,0,1,1,1,1,0,1,1,0,1,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,1,1,1,0,1,0,1,1,0,0,1,1,1,0,1,0,1,1,1,1,1,0,1,1,1,0,1,1,0,0,0,1,1,1,1,1,1,0,0,0,1,0,0,1,0,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,0,0,1,0,1,1,0,1,1,0,0,1,1,0,0,0,1,0,0,1,0,0,1,1,1,0,1,1,0,0,1,1,1,1,0,0,0,1,1,1,1,1,0,1,1,0,1,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,0,1,1,1,1,1,0,1,0,0,0,1,1,1,0,0,1,0,0,1,0,1,0,1,0,0,1,1,0,0,1,0,1,1,0,1,0,1,1,1,0,0,0,0,1,1,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,0,1,1,1,1,0,1,1,1,1,0,1,0,1,0,0,0,1,0,1,0,1,1,1,1,0,1,0,1,0,1,0,0,1,1,1,0,0,1,1,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,0,1,1,0,0,1,0,0,0,0,1,0,1,0,0,0,1,0,1,0,1,1,1,1,0,1,0,1,1,1,1,1,0,1,0,1,1,1,1,0,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,0,1,0,0,0,0,0,1,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,0,0,1,1,0,0,0,0,0,1,0,0,1,1,0,0,0,1,1,1,0,0,0,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,0,1,1,1,0,1,1,1,0,0,1,1,0,1,0,1,0,0,1,0,0,1,1,0,0,0,1,0,0,1,1,1,0,0,0,0,1,0,1,1,0,0,0,0,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,0,0,1,0,0,1,1,0,1,0,1,0,1,0,0,0,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1,0,0,0,0,1,0,1,0,1,1,1,1,1,1,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,0,0,1,0,0,1,0,1,0,1,1,1,1,0,1,0,0,0,0,1,1,0,0,1,0,0,0,1,0,1,0,0,1,0,0,1,0,0,0,0,0,1,1,1,0,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,0,1,1,0,0,1,0,1,1,0,1,1,1,1,0,1,0,0,1,1,1,1,0,1,1,0,0,0,1,0,0,1,0,1,0,1,1,0,0,0,1,0,0,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,1,0,1,0,0,0,1,1,1,0,1,0,1,0,0,0,1,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,1,1,0,0,0,1,0,0,1,1,1,1,0,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,0,0,1,0,0,1,1,0,0,1,0,0,1,0,0,1,1,1,1,1,0,0,0,0,0,1,1,0,1,0,1,0,0,0,1,0,0,0,0,1,1,0,0,0,0,0,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,0,1,0,0,1,1,0,0,0,1,0,0,0,0,1,1,1,1,0,1,1,0,1,0,0,0,0,0,0,1,1,1,1,1,1,0,1,1,1,0,0,1,0,1,0,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,0,1,0,0,1,0,1,1,1,0,1,0,0,0,1,0,1,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,1,0,0,0,1,1,0,1,1,1,1,1,0,0,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,1,1,1,1,0,0,0,1,0,0,0,0,0,1,0,0,0,1,1,0,0,0,1,0,1,1,1,1,1,1,0,0,0,1,0,1,0,0,0,1,0,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,1,0,0,1,0,1,0,1,0,1,0,1,1,1,0,1,0,0,0,0,1,0,0,1,1,1,1,1,0,0,1,0,1,1,0,0,0,0,1,0,1,1,1,0,0,1,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,0,0,1,1,1,0,0,0,0,1,1,0,1,0,0,1,1,0,1,1,1,1,0,0,0,1,1,0,1,0,0,1,0,1,0,0,1,0,0,0,1,1,1,0,0,0,1,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,0,0,0,0,1,1,0,0,0,1,0,0,1,1,0,1,0,1,0,0,1,0,1,1,0,0,0,1,1,0,0,0,0,1,1,1,1,1,0,1,1,0,0,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,1,1,0,0,1,0,0,1,1,1,1,0,1,1,0,1,1,1,0,0,1,0,1,1,1,1,1,1,1,1,1,1,0,1,1,0,0,1,0,0,0,0,0,1,1,0,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,0,0,0,0,0,1,1,0,1,1,0,0,1,1,0,1,1,1,0,0,0,1,0,1,1,1,1,0,1,0,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,1,0,0,0,0,0,0,1,0,1,1,1,0,1,0,0,0,1,1,1,0,0,0,1,1,0,1,0,1,0,1,0,0,0,0,0,1,0,1,1,1,1,1,1,1,0,0,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,1,0,1,0,0,1,0,1,0,1,0,1,0,0,0,0,0,1,1,0,1,0,1,0,1,0,1,1,1,1,0,1,1,0,0,1,1,1,0,0,0,0,0,1,0,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,1,1,1,0,1,0,0,0,1,1,0,0,1,1,1,1,0,1,1,1,1,0,0,1,1,1,0,1,1,1,1,1,1,1,0,0,0,1,0,0,0,0,0,0,1,0,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,0,0,1,0,1,0,1,1,1,0,1,1,0,0,0,0,1,0,0,1,0,1,1,0,0,1,1,0,0,1,0,0,1,0,1,1,0,0,0,1,1,0,0,1,0,1,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,0,1,1,0,0,0,1,1,1,1,1,1,1,0,1,0,1,1,0,1,1,1,1,1,1,0,1,1,1,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,1,0,0,1,0,1,0,1,0,1,1,0,0,0,0,1,0,1,0,1,1,1,0,1,0,0,0,0,0,1,1,0,0,1,0,1,0,0,1,0,0,0,0,0,0,1,0,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,0,1,0,1,0,1,1,1,1,0,1,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,1,0,0,0,1,0,0,1,0,0,1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,0,1,1,1,0,0,0,1,0,0,0,0,1,0,0,0,0,1,0,1,1,0,0,0,0,0,0,1,1,0,1,0,0,1,1,1,0,0,0,1,1,0,1,0,0,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,0,1,1,0,1,0,0,1,1,1,1,1,1,1,0,1,1,0,0,1,0,0,1,1,0,1,0,1,0,0,0,0,1,0,0,1,1,1,0,0,0,1,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,0,0,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,1,0,1,0,1,0,0,1,1,1,0,0,0,0,0,0,1,1,0,0,0,1,1,0,0,0,0,0,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,0,0,1,0,0,0,0,1,0,0,1,1,1,1,1,0,0,1,0,0,0,1,1,0,0,1,0,0,1,0,1,1,0,1,0,0,1,1,1,1,0,0,0,1,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,1,0,0,0,0,0,1,1,0,1,1,1,0,0,0,1,1,1,0,0,0,0,0,1,0,0,1,1,1,0,0,1,1,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,1,1,0,0,0,1,0,0,0,0,0,0,0,1,1,0,1,1,1,1,0,0,1,1,1,0,0,1,1,0,0,0,1,0,1,1,0,1,1,0,0,0,0,0,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,1,1,1,0,1,0,0,1,1,1,0,1,0,0,1,1,1,0,1,0,1,0,0,1,0,0,1,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,0,1,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,1,1,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,0,0,0,1,1,0,0,1,1,1,0,0,0,0,1,0,1,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,1,0,1,1,1,1,1,1,0,0,1,0,0,1,0,0,0,0,1,1,0,1,0,1,0,1,1,0,1,1,0,1,0,0,1,0,1,1,0,1,0,0,1,0,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,0,1,0,0,1,1,1,1,1,0,0,1,1,1,1,0,0,1,0,0,1,1,1,0,0,1,1,1,1,0,0,1,0,1,0,1,0,1,0,0,0,0,1,1,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,0,0,1,1,0,0,0,0,0,1,1,0,1,0,1,1,0,1,0,0,1,1,0,0,0,0,1,1,0,0,1,0,0,0,0,1,0,0,1,0,1,1,1,0,1,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,1,1,1,0,0,0,0,1,1,1,0,0,1,0,1,1,0,1,0,1,0,1,0,0,0,1,1,0,0,0,1,1,1,1,1,0,1,1,1,1,1,1,0,0,1,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,0,1,1,0,0,0,0,1,1,1,0,0,1,1,1,0,1,0,0,1,1,1,1,0,0,0,1,0,0,0,1,0,0,1,1,1,0,0,0,0,1,0,1,1,1,0,1,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,1,1,1,0,0,1,1,0,1,0,1,1,0,0,0,0,1,1,1,0,1,0,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,1,0,0,0,0,1,1,0,1,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,0,1,1,0,0,1,1,1,0,1,0,1,0,1,1,0,1,0,0,0,1,1,0,1,1,0,0,1,1,0,0,1,1,0,0,1,0,1,1,0,0,0,0,0,0,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,1,1,0,1,1,1,1,1,1,0,1,0,0,0,0,0,0,1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,1,0,1,0,0,0,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,1,0,0,1,0,1,1,0,0,1,1,0,1,0,0,0,1,0,1,1,1,1,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,1,1,0,1,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,1,0,1,0,1,0,0,1,1,0,0,0,0,1,1,0,0,1,0,0,0,0,1,0,0,0,1,0,0,0,1,1,0,1,0,0,1,1,0,1,1,0,0,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,0,1,0,0,1,1,1,1,1,1,0,0,1,1,1,1,0,1,1,1,1,0,1,0,0,0,0,0,0,1,1,0,1,1,0,0,1,0,1,1,0,0,1,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,1,1,1,0,0,1,0,0,0,0,1,1,1,0,0,0,0,1,0,0,0,0,1,0,1,0,0,1,1,1,1,1,1,1,1,0,1,1,1,1,1,1,0,0,1,1,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,1,0,0,1,1,1,1,0,1,1,1,0,0,1,0,1,1,0,1,1,0,1,1,0,1,0,0,0,1,0,0,0,1,1,1,1,0,0,0,0,0,1,1,1,0,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,1,0,1,0,1,0,1,0,1,0,1,1,1,0,1,1,0,1,1,0,1,0,1,0,1,0,1,0,0,0,1,0,0,1,1,0,0,1,0,1,1,0,1,1,1,1,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,1,1,0,1,1,0,1,0,0,1,1,0,0,0,1,1,1,1,1,1,0,0,0,1,0,1,0,1,1,0,0,0,1,1,1,0,1,0,0,0,1,0,1,1,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,0,1,0,0,0,1,1,1,0,1,1,0,1,0,0,0,0,0,0,1,0,0,1,1,0,1,1,0,0,1,0,0,0,0,1,1,1,1,0,0,1,1,0,1,0,0,0,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,0,1,1,1,1,0,0,1,1,0,0,0,1,0,1,1,0,0,1,0,0,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,1,0,0,1,1,0,1,0,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,0,0,1,0,0,1,1,0,0,0,0,1,1,1,0,1,0,0,0,1,0,1,0,1,1,0,0,1,0,1,1,0,1,1,0,1,0,1,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,0,1,0,0,1,0,1,0,1,0,1,1,1,0,0,1,0,0,1,1,0,1,1,0,0,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,0,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,1,1,0,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,1,0,0,0,1,1,0,1,0,0,0,1,1,0,0,1,0,0,1,0,0,0,1,0,0,0,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>WD10</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,0,1,1,1,1,0,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,1,0,1,1,1,1,0,1,1,1,1,1,1,1,1]</t>
   </si>
 </sst>
 </file>
@@ -534,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +885,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -572,98 +893,98 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -671,10 +992,10 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -682,10 +1003,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -693,10 +1014,10 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -704,10 +1025,10 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -715,10 +1036,10 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -726,10 +1047,10 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -737,10 +1058,10 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -748,10 +1069,10 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -759,10 +1080,10 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -770,10 +1091,10 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -781,10 +1102,10 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -792,10 +1113,10 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,10 +1124,10 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -814,10 +1135,10 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -825,136 +1146,532 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>44</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>45</v>
       </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C5" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
+  <autoFilter ref="A1:C73" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C73">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>